<commit_message>
Se agregó ServiciosProductos y se comprobó en postman. Funcional
</commit_message>
<xml_diff>
--- a/2_Rest_web_services_inventarios/inventarios.xlsx
+++ b/2_Rest_web_services_inventarios/inventarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_KRAKE_DEV\3_Tercer_modulo\2_Rest_web_services_inventarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1942475F-1526-49DD-96ED-47202A58CC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F1B20B-4620-4ECB-9C03-54DE88942711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AA63735-46FF-423B-8F2C-7519A2F63279}"/>
+    <workbookView xWindow="4080" yWindow="1725" windowWidth="14055" windowHeight="11280" activeTab="1" xr2:uid="{2AA63735-46FF-423B-8F2C-7519A2F63279}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -920,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D65A163-3162-4C9A-BE49-53DC9C7716AF}">
   <dimension ref="A2:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1779,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5110634E-C7BF-4911-A74B-12DC554BBA6F}">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se agregaron las entidades Pedido, Detalle Pedido y Estado Pedido, ademas de PEDIDOBDD y ServiciosPedidos
</commit_message>
<xml_diff>
--- a/2_Rest_web_services_inventarios/inventarios.xlsx
+++ b/2_Rest_web_services_inventarios/inventarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_KRAKE_DEV\3_Tercer_modulo\2_Rest_web_services_inventarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CCC54E-1464-4C26-955B-CE1F97B72E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24332F53-7C84-4C9C-9F00-453EC35B73F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1725" windowWidth="14055" windowHeight="11280" activeTab="1" xr2:uid="{2AA63735-46FF-423B-8F2C-7519A2F63279}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2AA63735-46FF-423B-8F2C-7519A2F63279}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="123">
   <si>
     <t>CODIGO</t>
   </si>
@@ -400,6 +400,12 @@
   </si>
   <si>
     <t>Crear un producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /pedidos/registrar</t>
+  </si>
+  <si>
+    <t>Crear un pedido</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +496,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -519,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -540,6 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -556,55 +569,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1027340</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>6804</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>458967</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>17055</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1599F1DF-6914-78E8-CE26-A7C5996901A4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6252483" y="768804"/>
-          <a:ext cx="2207484" cy="3248751"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -926,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D65A163-3162-4C9A-BE49-53DC9C7716AF}">
   <dimension ref="A2:I68"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,6 +1273,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
       <c r="B31" s="2" t="s">
         <v>113</v>
       </c>
@@ -1348,7 +1313,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
         <v>48</v>
       </c>
@@ -1368,12 +1333,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
       <c r="B36" s="2" t="s">
         <v>114</v>
       </c>
@@ -1381,7 +1347,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>51</v>
       </c>
@@ -1389,7 +1355,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>54</v>
       </c>
@@ -1397,7 +1363,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>66</v>
       </c>
@@ -1405,7 +1371,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>67</v>
       </c>
@@ -1425,7 +1391,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="6">
         <v>1</v>
       </c>
@@ -1435,18 +1401,18 @@
       <c r="D43" s="14">
         <v>45250</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="20" t="s">
         <v>78</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="6">
         <v>2</v>
       </c>
       <c r="C44" s="12" t="s">
@@ -1455,22 +1421,22 @@
       <c r="D44" s="14">
         <v>45250</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="20" t="s">
         <v>54</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>0</v>
       </c>
@@ -1490,7 +1456,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>1</v>
       </c>
@@ -1777,16 +1743,15 @@
     <hyperlink ref="F33" r:id="rId2" xr:uid="{F0F2978F-5E8C-4B7E-938A-5E8706869D2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5110634E-C7BF-4911-A74B-12DC554BBA6F}">
-  <dimension ref="B2:D7"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,6 +1825,17 @@
         <v>120</v>
       </c>
     </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agregaron los detalles de pedido dentro de la entidad PEDIDO. Se comprobaron en postman, todo OK
</commit_message>
<xml_diff>
--- a/2_Rest_web_services_inventarios/inventarios.xlsx
+++ b/2_Rest_web_services_inventarios/inventarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_KRAKE_DEV\3_Tercer_modulo\2_Rest_web_services_inventarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24332F53-7C84-4C9C-9F00-453EC35B73F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436C0F16-E4BE-49E3-8F76-6F1ADF96ED2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2AA63735-46FF-423B-8F2C-7519A2F63279}"/>
+    <workbookView xWindow="-28920" yWindow="2100" windowWidth="29040" windowHeight="15720" xr2:uid="{2AA63735-46FF-423B-8F2C-7519A2F63279}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -890,7 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D65A163-3162-4C9A-BE49-53DC9C7716AF}">
   <dimension ref="A2:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -1750,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5110634E-C7BF-4911-A74B-12DC554BBA6F}">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se agregó el PreparedStatement de la creación CabeceraVEnta. Se agregó el PreparedStatement de insertar Detalles
</commit_message>
<xml_diff>
--- a/2_Rest_web_services_inventarios/inventarios.xlsx
+++ b/2_Rest_web_services_inventarios/inventarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_KRAKE_DEV\3_Tercer_modulo\2_Rest_web_services_inventarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AC015A-D807-450F-A403-B128EC0C01E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8945D2EC-E1FB-4467-9346-FB18251FF337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2AA63735-46FF-423B-8F2C-7519A2F63279}"/>
+    <workbookView xWindow="5655" yWindow="1125" windowWidth="14055" windowHeight="11280" activeTab="1" xr2:uid="{2AA63735-46FF-423B-8F2C-7519A2F63279}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="128">
   <si>
     <t>CODIGO</t>
   </si>
@@ -415,6 +415,12 @@
   </si>
   <si>
     <t>Modifica el estado del pedido y de cada detalle actualiza la cantidad recibida y el subtotal</t>
+  </si>
+  <si>
+    <t>/ventas/guardar</t>
+  </si>
+  <si>
+    <t>Registra la cabecera y detalle de las ventas, además de los movimientos respectivos en el historial de stock</t>
   </si>
 </sst>
 </file>
@@ -1757,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5110634E-C7BF-4911-A74B-12DC554BBA6F}">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,6 +1862,17 @@
         <v>125</v>
       </c>
     </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>